<commit_message>
Google sheet logger update added
</commit_message>
<xml_diff>
--- a/Results/results.xlsx
+++ b/Results/results.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" iterate="0" iterateCount="100" iterateDelta="0.001" refMode="A1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="275">
   <si>
     <t>Date</t>
   </si>
@@ -837,6 +837,9 @@
   </si>
   <si>
     <t>Aug-17</t>
+  </si>
+  <si>
+    <t>16:50</t>
   </si>
 </sst>
 </file>
@@ -1255,7 +1258,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G864"/>
+  <dimension ref="A1:G865"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A235" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A255" activeCellId="0" pane="topLeft" sqref="A255:E255"/>
@@ -16997,6 +17000,23 @@
       </c>
       <c r="E864" t="n">
         <v>35.61</v>
+      </c>
+    </row>
+    <row r="865" spans="1:7">
+      <c r="A865" t="s">
+        <v>273</v>
+      </c>
+      <c r="B865" t="s">
+        <v>274</v>
+      </c>
+      <c r="C865" t="n">
+        <v>10.12</v>
+      </c>
+      <c r="D865" t="n">
+        <v>7.35</v>
+      </c>
+      <c r="E865" t="n">
+        <v>22.33</v>
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="1048576" s="6" spans="1:7"/>

</xml_diff>

<commit_message>
emailer and gspread update
</commit_message>
<xml_diff>
--- a/Results/results.xlsx
+++ b/Results/results.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" iterate="0" iterateCount="100" iterateDelta="0.001" refMode="A1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="284">
   <si>
     <t>Date</t>
   </si>
@@ -855,6 +855,18 @@
   </si>
   <si>
     <t>23:46</t>
+  </si>
+  <si>
+    <t>Aug-18</t>
+  </si>
+  <si>
+    <t>00:48</t>
+  </si>
+  <si>
+    <t>10:04</t>
+  </si>
+  <si>
+    <t>10:11</t>
   </si>
 </sst>
 </file>
@@ -1273,7 +1285,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G870"/>
+  <dimension ref="A1:G892"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A235" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A255" activeCellId="0" pane="topLeft" sqref="A255:E255"/>
@@ -17117,6 +17129,380 @@
       </c>
       <c r="E870" t="n">
         <v>18.17</v>
+      </c>
+    </row>
+    <row r="871" spans="1:7">
+      <c r="A871" t="s">
+        <v>280</v>
+      </c>
+      <c r="B871" t="s">
+        <v>281</v>
+      </c>
+      <c r="C871" t="n">
+        <v>9.57</v>
+      </c>
+      <c r="D871" t="n">
+        <v>10.51</v>
+      </c>
+      <c r="E871" t="n">
+        <v>38.06</v>
+      </c>
+    </row>
+    <row r="872" spans="1:7">
+      <c r="A872" t="s">
+        <v>280</v>
+      </c>
+      <c r="B872" t="s">
+        <v>37</v>
+      </c>
+      <c r="C872" t="n">
+        <v>9.26</v>
+      </c>
+      <c r="D872" t="n">
+        <v>10.43</v>
+      </c>
+      <c r="E872" t="n">
+        <v>33.98</v>
+      </c>
+    </row>
+    <row r="873" spans="1:7">
+      <c r="A873" t="s">
+        <v>280</v>
+      </c>
+      <c r="B873" t="s">
+        <v>38</v>
+      </c>
+      <c r="C873" t="n">
+        <v>9.59</v>
+      </c>
+      <c r="D873" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="E873" t="n">
+        <v>36.28</v>
+      </c>
+    </row>
+    <row r="874" spans="1:7">
+      <c r="A874" t="s">
+        <v>280</v>
+      </c>
+      <c r="B874" t="s">
+        <v>52</v>
+      </c>
+      <c r="C874" t="n">
+        <v>9.94</v>
+      </c>
+      <c r="D874" t="n">
+        <v>10.41</v>
+      </c>
+      <c r="E874" t="n">
+        <v>33.45</v>
+      </c>
+    </row>
+    <row r="875" spans="1:7">
+      <c r="A875" t="s">
+        <v>280</v>
+      </c>
+      <c r="B875" t="s">
+        <v>53</v>
+      </c>
+      <c r="C875" t="n">
+        <v>10.37</v>
+      </c>
+      <c r="D875" t="n">
+        <v>10.02</v>
+      </c>
+      <c r="E875" t="n">
+        <v>34.8</v>
+      </c>
+    </row>
+    <row r="876" spans="1:7">
+      <c r="A876" t="s">
+        <v>280</v>
+      </c>
+      <c r="B876" t="s">
+        <v>54</v>
+      </c>
+      <c r="C876" t="n">
+        <v>10.33</v>
+      </c>
+      <c r="D876" t="n">
+        <v>9.630000000000001</v>
+      </c>
+      <c r="E876" t="n">
+        <v>36.44</v>
+      </c>
+    </row>
+    <row r="877" spans="1:7">
+      <c r="A877" t="s">
+        <v>280</v>
+      </c>
+      <c r="B877" t="s">
+        <v>55</v>
+      </c>
+      <c r="C877" t="n">
+        <v>9.960000000000001</v>
+      </c>
+      <c r="D877" t="n">
+        <v>9.82</v>
+      </c>
+      <c r="E877" t="n">
+        <v>38.03</v>
+      </c>
+    </row>
+    <row r="878" spans="1:7">
+      <c r="A878" t="s">
+        <v>280</v>
+      </c>
+      <c r="B878" t="s">
+        <v>56</v>
+      </c>
+      <c r="C878" t="n">
+        <v>10.36</v>
+      </c>
+      <c r="D878" t="n">
+        <v>10.71</v>
+      </c>
+      <c r="E878" t="n">
+        <v>34.61</v>
+      </c>
+    </row>
+    <row r="879" spans="1:7">
+      <c r="A879" t="s">
+        <v>280</v>
+      </c>
+      <c r="B879" t="s">
+        <v>57</v>
+      </c>
+      <c r="C879" t="n">
+        <v>10.35</v>
+      </c>
+      <c r="D879" t="n">
+        <v>10.59</v>
+      </c>
+      <c r="E879" t="n">
+        <v>37.2</v>
+      </c>
+    </row>
+    <row r="880" spans="1:7">
+      <c r="A880" t="s">
+        <v>280</v>
+      </c>
+      <c r="B880" t="s">
+        <v>58</v>
+      </c>
+      <c r="C880" t="n">
+        <v>10.35</v>
+      </c>
+      <c r="D880" t="n">
+        <v>10.68</v>
+      </c>
+      <c r="E880" t="n">
+        <v>34.74</v>
+      </c>
+    </row>
+    <row r="881" spans="1:7">
+      <c r="A881" t="s">
+        <v>280</v>
+      </c>
+      <c r="B881" t="s">
+        <v>59</v>
+      </c>
+      <c r="C881" t="n">
+        <v>10.33</v>
+      </c>
+      <c r="D881" t="n">
+        <v>10.69</v>
+      </c>
+      <c r="E881" t="n">
+        <v>32.94</v>
+      </c>
+    </row>
+    <row r="882" spans="1:7">
+      <c r="A882" t="s">
+        <v>280</v>
+      </c>
+      <c r="B882" t="s">
+        <v>60</v>
+      </c>
+      <c r="C882" t="n">
+        <v>9.73</v>
+      </c>
+      <c r="D882" t="n">
+        <v>10.51</v>
+      </c>
+      <c r="E882" t="n">
+        <v>37.97</v>
+      </c>
+    </row>
+    <row r="883" spans="1:7">
+      <c r="A883" t="s">
+        <v>280</v>
+      </c>
+      <c r="B883" t="s">
+        <v>61</v>
+      </c>
+      <c r="C883" t="n">
+        <v>10.31</v>
+      </c>
+      <c r="D883" t="n">
+        <v>10.69</v>
+      </c>
+      <c r="E883" t="n">
+        <v>32.26</v>
+      </c>
+    </row>
+    <row r="884" spans="1:7">
+      <c r="A884" t="s">
+        <v>280</v>
+      </c>
+      <c r="B884" t="s">
+        <v>62</v>
+      </c>
+      <c r="C884" t="n">
+        <v>10.36</v>
+      </c>
+      <c r="D884" t="n">
+        <v>9.609999999999999</v>
+      </c>
+      <c r="E884" t="n">
+        <v>33.17</v>
+      </c>
+    </row>
+    <row r="885" spans="1:7">
+      <c r="A885" t="s">
+        <v>280</v>
+      </c>
+      <c r="B885" t="s">
+        <v>63</v>
+      </c>
+      <c r="C885" t="n">
+        <v>10.17</v>
+      </c>
+      <c r="D885" t="n">
+        <v>10.61</v>
+      </c>
+      <c r="E885" t="n">
+        <v>32.17</v>
+      </c>
+    </row>
+    <row r="886" spans="1:7">
+      <c r="A886" t="s">
+        <v>280</v>
+      </c>
+      <c r="B886" t="s">
+        <v>64</v>
+      </c>
+      <c r="C886" t="n">
+        <v>10.33</v>
+      </c>
+      <c r="D886" t="n">
+        <v>10.47</v>
+      </c>
+      <c r="E886" t="n">
+        <v>35.91</v>
+      </c>
+    </row>
+    <row r="887" spans="1:7">
+      <c r="A887" t="s">
+        <v>280</v>
+      </c>
+      <c r="B887" t="s">
+        <v>65</v>
+      </c>
+      <c r="C887" t="n">
+        <v>7.27</v>
+      </c>
+      <c r="D887" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="E887" t="n">
+        <v>40.96</v>
+      </c>
+    </row>
+    <row r="888" spans="1:7">
+      <c r="A888" t="s">
+        <v>280</v>
+      </c>
+      <c r="B888" t="s">
+        <v>66</v>
+      </c>
+      <c r="C888" t="n">
+        <v>9.529999999999999</v>
+      </c>
+      <c r="D888" t="n">
+        <v>9.99</v>
+      </c>
+      <c r="E888" t="n">
+        <v>34.75</v>
+      </c>
+    </row>
+    <row r="889" spans="1:7">
+      <c r="A889" t="s">
+        <v>280</v>
+      </c>
+      <c r="B889" t="s">
+        <v>67</v>
+      </c>
+      <c r="C889" t="n">
+        <v>9.470000000000001</v>
+      </c>
+      <c r="D889" t="n">
+        <v>4.68</v>
+      </c>
+      <c r="E889" t="n">
+        <v>50.03</v>
+      </c>
+    </row>
+    <row r="890" spans="1:7">
+      <c r="A890" t="s">
+        <v>280</v>
+      </c>
+      <c r="B890" t="s">
+        <v>68</v>
+      </c>
+      <c r="C890" t="n">
+        <v>10.31</v>
+      </c>
+      <c r="D890" t="n">
+        <v>10.33</v>
+      </c>
+      <c r="E890" t="n">
+        <v>46.17</v>
+      </c>
+    </row>
+    <row r="891" spans="1:7">
+      <c r="A891" t="s">
+        <v>280</v>
+      </c>
+      <c r="B891" t="s">
+        <v>282</v>
+      </c>
+      <c r="C891" t="n">
+        <v>10.3</v>
+      </c>
+      <c r="D891" t="n">
+        <v>9.630000000000001</v>
+      </c>
+      <c r="E891" t="n">
+        <v>34.71</v>
+      </c>
+    </row>
+    <row r="892" spans="1:7">
+      <c r="A892" t="s">
+        <v>280</v>
+      </c>
+      <c r="B892" t="s">
+        <v>283</v>
+      </c>
+      <c r="C892" t="n">
+        <v>6</v>
+      </c>
+      <c r="D892" t="n">
+        <v>10</v>
+      </c>
+      <c r="E892" t="n">
+        <v>20</v>
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="1048576" s="6" spans="1:7"/>

</xml_diff>

<commit_message>
results update while testing
</commit_message>
<xml_diff>
--- a/Results/results.xlsx
+++ b/Results/results.xlsx
@@ -1285,7 +1285,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G892"/>
+  <dimension ref="A1:G894"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A235" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A255" activeCellId="0" pane="topLeft" sqref="A255:E255"/>
@@ -17502,6 +17502,40 @@
         <v>10</v>
       </c>
       <c r="E892" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="893" spans="1:7">
+      <c r="A893" t="s">
+        <v>280</v>
+      </c>
+      <c r="B893" t="s">
+        <v>69</v>
+      </c>
+      <c r="C893" t="n">
+        <v>6</v>
+      </c>
+      <c r="D893" t="n">
+        <v>10</v>
+      </c>
+      <c r="E893" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="894" spans="1:7">
+      <c r="A894" t="s">
+        <v>280</v>
+      </c>
+      <c r="B894" t="s">
+        <v>70</v>
+      </c>
+      <c r="C894" t="n">
+        <v>6</v>
+      </c>
+      <c r="D894" t="n">
+        <v>10</v>
+      </c>
+      <c r="E894" t="n">
         <v>20</v>
       </c>
     </row>

</xml_diff>